<commit_message>
fix: minor change for preSettings; test: add more for preSettings;
</commit_message>
<xml_diff>
--- a/tools/data-processing/taverns.xlsx
+++ b/tools/data-processing/taverns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\might-and-magic\arcomage-hd\tools\data-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675989B5-0318-44E2-894E-02E8E8401F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7023794-BBEE-4EAC-AF5B-7F1C2AEE1316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1053,7 +1053,7 @@
     <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" customWidth="1"/>
     <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.5546875" bestFit="1" customWidth="1"/>
@@ -2607,10 +2607,10 @@
         <v>203</v>
       </c>
       <c r="F29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -2641,7 +2641,7 @@
       </c>
       <c r="R29" t="str">
         <f>F29&amp;G29&amp;H29&amp;I29&amp;J29&amp;K29&amp;L29&amp;M29&amp;N29&amp;O29&amp;P29</f>
-        <v>991110001252503</v>
+        <v>10101110001252503</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -2745,10 +2745,10 @@
     <cfRule type="duplicateValues" dxfId="3" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R1048576 R1:R31">
-    <cfRule type="duplicateValues" dxfId="1" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R33:R1048576 R26:R31 R1:R14">
-    <cfRule type="duplicateValues" dxfId="0" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="19"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4092,7 +4092,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q1:Q1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix: better preSettings for mm6
</commit_message>
<xml_diff>
--- a/tools/data-processing/taverns.xlsx
+++ b/tools/data-processing/taverns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chen\githubprojects\might-and-magic\arcomage-hd\tools\data-processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7023794-BBEE-4EAC-AF5B-7F1C2AEE1316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A535B3-7CB2-456D-A336-0AFA205C2420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,9 +641,6 @@
     <t>Misty Islands</t>
   </si>
   <si>
-    <t>Freehaven</t>
-  </si>
-  <si>
     <t>Frozen Highlands</t>
   </si>
   <si>
@@ -665,10 +662,13 @@
     <t>Lady Loretta Fleise</t>
   </si>
   <si>
-    <t>Lord Erik Von Stromgard</t>
-  </si>
-  <si>
     <t>Prince Nicolai Ironfist</t>
+  </si>
+  <si>
+    <t>Free Haven</t>
+  </si>
+  <si>
+    <t>Lord Erik von Stromgard</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1045,7 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,7 +1072,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D1" t="s">
         <v>172</v>
@@ -1170,7 +1170,7 @@
         <v>177</v>
       </c>
       <c r="R2" t="str">
-        <f>F2&amp;G2&amp;H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2</f>
+        <f t="shared" ref="R2:R31" si="0">F2&amp;G2&amp;H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2</f>
         <v>155222101010301005</v>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
         <v>179</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" ref="R3:R25" si="0">F3&amp;G3&amp;H3&amp;I3&amp;J3&amp;K3&amp;L3&amp;M3&amp;N3&amp;O3&amp;P3</f>
+        <f t="shared" si="0"/>
         <v>205222555501505</v>
       </c>
     </row>
@@ -2457,10 +2457,10 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E26" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="F26">
         <v>25</v>
@@ -2487,17 +2487,17 @@
         <v>10</v>
       </c>
       <c r="N26">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="O26">
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="P26">
         <v>6</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" ref="R26:R27" si="1">F26&amp;G26&amp;H26&amp;I26&amp;J26&amp;K26&amp;L26&amp;M26&amp;N26&amp;O26&amp;P26</f>
-        <v>25304441010102004506</v>
+        <f t="shared" si="0"/>
+        <v>25304441010101755006</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
@@ -2505,10 +2505,10 @@
         <v>6</v>
       </c>
       <c r="D27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F27">
         <v>40</v>
@@ -2544,7 +2544,7 @@
         <v>4</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40405522025101254504</v>
       </c>
     </row>
@@ -2553,10 +2553,10 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E28" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F28">
         <v>30</v>
@@ -2583,7 +2583,7 @@
         <v>30</v>
       </c>
       <c r="N28">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="O28">
         <v>500</v>
@@ -2592,8 +2592,8 @@
         <v>4</v>
       </c>
       <c r="R28" t="str">
-        <f>F28&amp;G28&amp;H28&amp;I28&amp;J28&amp;K28&amp;L28&amp;M28&amp;N28&amp;O28&amp;P28</f>
-        <v>305011555302005004</v>
+        <f t="shared" si="0"/>
+        <v>305011555301505004</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -2601,10 +2601,10 @@
         <v>6</v>
       </c>
       <c r="D29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F29">
         <v>10</v>
@@ -2640,7 +2640,7 @@
         <v>3</v>
       </c>
       <c r="R29" t="str">
-        <f>F29&amp;G29&amp;H29&amp;I29&amp;J29&amp;K29&amp;L29&amp;M29&amp;N29&amp;O29&amp;P29</f>
+        <f t="shared" si="0"/>
         <v>10101110001252503</v>
       </c>
     </row>
@@ -2649,7 +2649,7 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E30" t="s">
         <v>200</v>
@@ -2679,17 +2679,17 @@
         <v>5</v>
       </c>
       <c r="N30">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="O30">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="P30">
         <v>4</v>
       </c>
       <c r="R30" t="str">
-        <f>F30&amp;G30&amp;H30&amp;I30&amp;J30&amp;K30&amp;L30&amp;M30&amp;N30&amp;O30&amp;P30</f>
-        <v>55016154054005504</v>
+        <f t="shared" si="0"/>
+        <v>55016154052006004</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -2697,7 +2697,7 @@
         <v>6</v>
       </c>
       <c r="D31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E31" t="s">
         <v>194</v>
@@ -2727,7 +2727,7 @@
         <v>25</v>
       </c>
       <c r="N31">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="O31">
         <v>750</v>
@@ -2736,8 +2736,8 @@
         <v>7</v>
       </c>
       <c r="R31" t="str">
-        <f>F31&amp;G31&amp;H31&amp;I31&amp;J31&amp;K31&amp;L31&amp;M31&amp;N31&amp;O31&amp;P31</f>
-        <v>60605552525255007507</v>
+        <f t="shared" si="0"/>
+        <v>60605552525252507507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>